<commit_message>
Se puso dueño a la base COL2021 y peces
</commit_message>
<xml_diff>
--- a/Usuarios_servidor_puma.xlsx
+++ b/Usuarios_servidor_puma.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\portuno\github_local\usuarios_servidor_puma-mdb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="386">
   <si>
     <t>nombre usuario</t>
   </si>
@@ -1633,11 +1638,14 @@
   <si>
     <t>Victor Vargas</t>
   </si>
+  <si>
+    <t>Axel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1953,7 +1961,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1988,7 +1996,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3949,7 +3957,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,6 +3994,9 @@
       <c r="A4" t="s">
         <v>344</v>
       </c>
+      <c r="B4" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4038,6 +4049,9 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>350</v>
+      </c>
+      <c r="B11" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>